<commit_message>
Added all the html pages
</commit_message>
<xml_diff>
--- a/data/Student and Faculty Commons Survey_February 16, 2022_09.17.xlsx
+++ b/data/Student and Faculty Commons Survey_February 16, 2022_09.17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianmasse/Developer/Classes/CSC630/group-work/Commons-Data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC43F47-B8F2-1842-B815-34BE9D6D41B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D0C7D7-DB22-9649-8E5E-D718563B6F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="228">
   <si>
     <t>StartDate</t>
   </si>
@@ -698,6 +698,24 @@
   </si>
   <si>
     <t>sexuality</t>
+  </si>
+  <si>
+    <t>Socio economic class</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Dietary restrictions</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Lunch period</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1539,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD16"/>
+  <dimension ref="A1:BG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="BD5" sqref="BD5"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="BC8" sqref="BC8:BD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1568,7 @@
     <col min="1" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>21</v>
+        <v>227</v>
       </c>
       <c r="AA1" t="s">
         <v>25</v>
@@ -1708,7 +1726,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1866,7 +1884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -2024,7 +2042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44604.385601851849</v>
       </c>
@@ -2071,7 +2089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44604.390590277777</v>
       </c>
@@ -2111,8 +2129,14 @@
       <c r="R5" t="s">
         <v>152</v>
       </c>
+      <c r="BC5" t="s">
+        <v>222</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44604.391817129632</v>
       </c>
@@ -2155,8 +2179,14 @@
       <c r="S6" t="s">
         <v>155</v>
       </c>
+      <c r="BC6" t="s">
+        <v>223</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44604.429224537038</v>
       </c>
@@ -2283,8 +2313,14 @@
       <c r="AX7" t="s">
         <v>174</v>
       </c>
+      <c r="BC7" t="s">
+        <v>224</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44605.398090277777</v>
       </c>
@@ -2324,8 +2360,14 @@
       <c r="Q8" t="s">
         <v>148</v>
       </c>
+      <c r="BC8" t="s">
+        <v>225</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44606.317962962959</v>
       </c>
@@ -2453,7 +2495,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44606.326412037037</v>
       </c>
@@ -2491,7 +2533,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44606.439814814818</v>
       </c>
@@ -2619,7 +2661,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44606.440104166664</v>
       </c>
@@ -2732,7 +2774,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44606.443171296298</v>
       </c>
@@ -2859,8 +2901,14 @@
       <c r="AX13" t="s">
         <v>200</v>
       </c>
+      <c r="BF13" t="s">
+        <v>226</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44608.351921296293</v>
       </c>
@@ -2898,7 +2946,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44608.35491898148</v>
       </c>
@@ -2954,7 +3002,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44608.378680555557</v>
       </c>

</xml_diff>